<commit_message>
small change to PRISMA
Need to delete the grey boxes
</commit_message>
<xml_diff>
--- a/data/LSR2_H_PRISMA_100344.xlsx
+++ b/data/LSR2_H_PRISMA_100344.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Desktop\Github rep\LSR2_exercise_H\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D705F3-C3CD-47A2-9F2F-A636595FCD3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE67C5F-E43F-4AB5-BDCB-8EB3D6C863C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="912" yWindow="204" windowWidth="19380" windowHeight="12180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LSR2_H_PRISMA_210.03.44" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="154">
   <si>
     <t>data</t>
   </si>
@@ -169,9 +169,6 @@
     <t>Identification of new studies via other methods</t>
   </si>
   <si>
-    <t>othstud.html</t>
-  </si>
-  <si>
     <t>website_results</t>
   </si>
   <si>
@@ -187,12 +184,6 @@
     <t>Websites</t>
   </si>
   <si>
-    <t>Records identified from: Websites, Organisations and Citation Searching</t>
-  </si>
-  <si>
-    <t>website_results.html</t>
-  </si>
-  <si>
     <t>organisation_results</t>
   </si>
   <si>
@@ -322,12 +313,6 @@
     <t>Reports sought for retrieval (other)</t>
   </si>
   <si>
-    <t>other_sought_reports.html</t>
-  </si>
-  <si>
-    <t>missing full text, 11</t>
-  </si>
-  <si>
     <t>other_notretrieved_reports</t>
   </si>
   <si>
@@ -340,9 +325,6 @@
     <t>Reports not retrieved (other)</t>
   </si>
   <si>
-    <t>other_notretrieved_reports.html</t>
-  </si>
-  <si>
     <t>dbr_assessed</t>
   </si>
   <si>
@@ -397,9 +379,6 @@
     <t>Reports assessed for eligibility (other)</t>
   </si>
   <si>
-    <t>other_assessed.html</t>
-  </si>
-  <si>
     <t>other_excluded</t>
   </si>
   <si>
@@ -410,12 +389,6 @@
   </si>
   <si>
     <t>Reports excluded (other): [separate reasons and numbers using ; e.g. Reason1, xxx; Reason2, xxx; Reason3, xxx]</t>
-  </si>
-  <si>
-    <t>Reports excluded (other)</t>
-  </si>
-  <si>
-    <t>other_excluded.html</t>
   </si>
   <si>
     <t>new_studies</t>
@@ -651,7 +624,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -829,6 +802,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -992,8 +971,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1372,10 +1352,16 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M15:M16"/>
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="25.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.21875" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1628,10 +1614,10 @@
         <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -1639,25 +1625,25 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
         <v>50</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>52</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>53</v>
       </c>
-      <c r="E11" t="s">
-        <v>54</v>
-      </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1665,16 +1651,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
         <v>8</v>
@@ -1688,19 +1674,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>8</v>
@@ -1714,25 +1700,25 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="B14" t="s">
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G14" t="s">
-        <v>67</v>
       </c>
       <c r="H14">
         <v>4784</v>
@@ -1740,19 +1726,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E15" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" t="s">
         <v>8</v>
@@ -1766,19 +1752,19 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F16" t="s">
         <v>8</v>
@@ -1792,25 +1778,25 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" t="s">
         <v>72</v>
       </c>
-      <c r="B17" t="s">
+      <c r="E17" t="s">
         <v>73</v>
       </c>
-      <c r="C17" t="s">
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" t="s">
         <v>74</v>
-      </c>
-      <c r="D17" t="s">
-        <v>75</v>
-      </c>
-      <c r="E17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" t="s">
-        <v>77</v>
       </c>
       <c r="H17">
         <v>7086</v>
@@ -1818,25 +1804,25 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
         <v>78</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>79</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" t="s">
         <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G18" t="s">
-        <v>83</v>
       </c>
       <c r="H18">
         <v>6914</v>
@@ -1844,25 +1830,25 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
         <v>84</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>85</v>
       </c>
-      <c r="C19" t="s">
+      <c r="F19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" t="s">
         <v>86</v>
-      </c>
-      <c r="D19" t="s">
-        <v>87</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" t="s">
-        <v>89</v>
       </c>
       <c r="H19">
         <v>172</v>
@@ -1870,25 +1856,25 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
+      <c r="E20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s">
+      <c r="F20" t="s">
+        <v>90</v>
+      </c>
+      <c r="G20" t="s">
         <v>92</v>
-      </c>
-      <c r="D20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E20" t="s">
-        <v>94</v>
-      </c>
-      <c r="F20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G20" t="s">
-        <v>95</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -1896,51 +1882,51 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" t="s">
         <v>96</v>
       </c>
-      <c r="B21" t="s">
-        <v>97</v>
-      </c>
-      <c r="C21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D21" t="s">
-        <v>99</v>
-      </c>
       <c r="E21" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F21" t="s">
-        <v>99</v>
+        <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
-      </c>
-      <c r="H21" t="s">
-        <v>101</v>
+        <v>8</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B22" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C22" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D22" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F22" t="s">
-        <v>105</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>106</v>
+        <v>8</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -1948,25 +1934,25 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="D23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="E23" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="G23" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="H23">
         <v>161</v>
@@ -1974,51 +1960,51 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" t="s">
+        <v>111</v>
+      </c>
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" t="s">
         <v>113</v>
       </c>
-      <c r="B24" t="s">
+      <c r="H24" t="s">
         <v>114</v>
-      </c>
-      <c r="C24" t="s">
-        <v>115</v>
-      </c>
-      <c r="D24" t="s">
-        <v>116</v>
-      </c>
-      <c r="E24" t="s">
-        <v>117</v>
-      </c>
-      <c r="F24" t="s">
-        <v>118</v>
-      </c>
-      <c r="G24" t="s">
-        <v>119</v>
-      </c>
-      <c r="H24" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>124</v>
+        <v>8</v>
       </c>
       <c r="G25" t="s">
-        <v>125</v>
+        <v>8</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -2026,25 +2012,25 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B26" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C26" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D26" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F26" t="s">
-        <v>130</v>
+        <v>8</v>
       </c>
       <c r="G26" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2052,25 +2038,25 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E27" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F27" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="G27" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="H27">
         <v>44</v>
@@ -2078,19 +2064,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="E28" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F28" t="s">
         <v>8</v>
@@ -2104,25 +2090,25 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C29" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D29" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E29" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="F29" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="G29" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2130,19 +2116,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E30" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F30" t="s">
         <v>8</v>
@@ -2154,81 +2140,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+    <row r="31" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B31" t="s">
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="C31" t="s">
-        <v>148</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="B33" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="E31" t="s">
+      <c r="C33" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="F31" t="s">
-        <v>150</v>
-      </c>
-      <c r="G31" t="s">
+      <c r="E33" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="F33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="B32" t="s">
-        <v>154</v>
-      </c>
-      <c r="C32" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" t="s">
-        <v>155</v>
-      </c>
-      <c r="G32" t="s">
-        <v>157</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>158</v>
-      </c>
-      <c r="B33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C33" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" t="s">
-        <v>160</v>
-      </c>
-      <c r="E33" t="s">
-        <v>161</v>
-      </c>
-      <c r="F33" t="s">
-        <v>160</v>
-      </c>
-      <c r="G33" t="s">
-        <v>162</v>
-      </c>
-      <c r="H33">
+      <c r="H33" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>